<commit_message>
20210722 CRE20-015-13	Add additional information to SSSCMC raw data report (Phase 13)
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-0XX (HA Scheme)\Front-end (Phase 10 - SP &amp; Back-office claim)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-015 (HA Scheme)\Front-end (Phase 13 - Enhance eHSU0015 raw data report)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Change History" sheetId="31" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AA$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AD$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -77,28 +77,10 @@
     <t>Doc. No.</t>
   </si>
   <si>
-    <t>全額減免病人</t>
-  </si>
-  <si>
     <t>病人申请费用减免资料不符</t>
   </si>
   <si>
     <t>病人自付费用 ¥</t>
-  </si>
-  <si>
-    <t>診金¥</t>
-  </si>
-  <si>
-    <t>藥費¥</t>
-  </si>
-  <si>
-    <t>檢驗費¥</t>
-  </si>
-  <si>
-    <t>其他費用¥</t>
-  </si>
-  <si>
-    <t>其他費用-注明</t>
   </si>
   <si>
     <t>总服务费用¥ (至角)</t>
@@ -176,6 +158,46 @@
   </si>
   <si>
     <t>2. Columns description reference to the claim page</t>
+  </si>
+  <si>
+    <t>Name (English)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name (Chinese)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add additional information to SSSCMC raw data report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验费¥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>全额減免病人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>诊金¥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>药费¥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他费用¥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他费用-注明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -188,7 +210,7 @@
     <numFmt numFmtId="178" formatCode="0_ "/>
     <numFmt numFmtId="179" formatCode="[$-13C09]d\ mmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -256,6 +278,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="HA_MingLiu"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +319,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -453,6 +481,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -482,19 +516,19 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>261196</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>189814</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>89087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -505,18 +539,29 @@
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="862853"/>
-          <a:ext cx="8900931" cy="6565961"/>
+          <a:off x="0" y="874059"/>
+          <a:ext cx="8896910" cy="6666940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -832,10 +877,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -857,7 +902,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
@@ -873,29 +918,32 @@
     <col min="5" max="5" width="11.375" style="22" customWidth="1"/>
     <col min="6" max="6" width="9" style="27" customWidth="1"/>
     <col min="7" max="7" width="12.375" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="10.625" style="29" customWidth="1"/>
-    <col min="11" max="13" width="10.5" style="29" customWidth="1"/>
-    <col min="14" max="14" width="13.25" style="29" customWidth="1"/>
-    <col min="15" max="15" width="9" style="27" customWidth="1"/>
-    <col min="16" max="16" width="12.75" style="29" customWidth="1"/>
-    <col min="17" max="17" width="20.875" style="19" customWidth="1"/>
-    <col min="18" max="18" width="15.75" style="19" customWidth="1"/>
-    <col min="19" max="19" width="17.375" style="19" customWidth="1"/>
-    <col min="20" max="20" width="10.625" style="19" customWidth="1"/>
-    <col min="21" max="21" width="14" style="19" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="19" customWidth="1"/>
-    <col min="23" max="23" width="20.5" style="19" customWidth="1"/>
-    <col min="24" max="24" width="12.875" style="40" customWidth="1"/>
-    <col min="25" max="25" width="15.75" style="38" customWidth="1"/>
-    <col min="26" max="26" width="15.875" style="20" customWidth="1"/>
-    <col min="27" max="27" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="27" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="55" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" style="27" customWidth="1"/>
+    <col min="12" max="12" width="9.625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="29" customWidth="1"/>
+    <col min="14" max="16" width="10.5" style="29" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="29" customWidth="1"/>
+    <col min="18" max="18" width="9" style="27" customWidth="1"/>
+    <col min="19" max="19" width="12.75" style="29" customWidth="1"/>
+    <col min="20" max="20" width="20.875" style="19" customWidth="1"/>
+    <col min="21" max="21" width="15.75" style="19" customWidth="1"/>
+    <col min="22" max="22" width="17.375" style="19" customWidth="1"/>
+    <col min="23" max="23" width="10.625" style="19" customWidth="1"/>
+    <col min="24" max="24" width="14" style="19" customWidth="1"/>
+    <col min="25" max="25" width="11.625" style="19" customWidth="1"/>
+    <col min="26" max="26" width="20.5" style="19" customWidth="1"/>
+    <col min="27" max="27" width="12.875" style="40" customWidth="1"/>
+    <col min="28" max="28" width="15.75" style="38" customWidth="1"/>
+    <col min="29" max="29" width="15.875" style="20" customWidth="1"/>
+    <col min="30" max="30" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -903,51 +951,60 @@
       <c r="E1" s="51"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
-      <c r="O1" s="16"/>
+      <c r="O1" s="18"/>
       <c r="P1" s="18"/>
-    </row>
-    <row r="2" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="18"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="18"/>
+    </row>
+    <row r="2" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="42"/>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
-      <c r="O2" s="23"/>
+      <c r="O2" s="25"/>
       <c r="P2" s="25"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="25"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" s="42"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="24"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
-      <c r="O3" s="23"/>
+      <c r="O3" s="25"/>
       <c r="P3" s="25"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Q3" s="25"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="25"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="48"/>
@@ -955,29 +1012,35 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
-      <c r="O4" s="16"/>
+      <c r="O4" s="18"/>
       <c r="P4" s="18"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="18"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="22"/>
+      <c r="L5" s="24"/>
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
-      <c r="O5" s="23"/>
+      <c r="O5" s="25"/>
       <c r="P5" s="25"/>
-    </row>
-    <row r="6" spans="1:27" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="25"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="25"/>
+    </row>
+    <row r="6" spans="1:30" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>3</v>
       </c>
@@ -991,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>12</v>
@@ -999,73 +1062,85 @@
       <c r="G6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="M6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="N6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="T6" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="X6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="30" t="s">
+      <c r="AC6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="T6" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="U6" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="V6" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="41" t="s">
+      <c r="AD6" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="Y6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z6" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA6" s="37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AA6"/>
+  <autoFilter ref="A6:AD6"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1086,19 +1161,19 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3"/>
     </row>
@@ -1271,7 +1346,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1315,13 +1390,27 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10">
         <v>44180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210726 CRE20-015-14	Add additional information to SSSCMC raw data report (Phase 14)
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-015 (HA Scheme)\Front-end (Phase 13 - Enhance eHSU0015 raw data report)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-015 (HA Scheme)\Front-end (Phase 14 - Enhance eHSU0015 raw data report)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Change History" sheetId="31" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AD$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AF$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -197,6 +197,66 @@
   </si>
   <si>
     <t>其他费用-注明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Exact date DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>MM/YYYY</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Only year YYYY</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Exemption Certificate: Date of registration + age</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Exemption Certificate: Reported year of birth</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Exemption Certificate: Exact date DD/MM/YYYY on travel document   HKBC: Exact date DD/MM/YYYY for DOB in word</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Exemption Certificate: MM/YYYY on travel document   HKBC: MM/YYYY for DOB in word</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Exemption Certificate: Only year YYYY on travel document   HKBC: Only year YYYY for DOB in word</t>
+  </si>
+  <si>
+    <t>3. Date of Birth Flag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date of Birth Flag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -319,7 +379,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -487,6 +547,27 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -902,7 +983,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
@@ -920,28 +1001,30 @@
     <col min="7" max="7" width="12.375" style="27" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="27" customWidth="1"/>
     <col min="9" max="9" width="14.5" style="55" customWidth="1"/>
-    <col min="10" max="10" width="6.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" style="27" customWidth="1"/>
-    <col min="12" max="12" width="9.625" style="28" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="29" customWidth="1"/>
-    <col min="14" max="16" width="10.5" style="29" customWidth="1"/>
-    <col min="17" max="17" width="13.25" style="29" customWidth="1"/>
-    <col min="18" max="18" width="9" style="27" customWidth="1"/>
-    <col min="19" max="19" width="12.75" style="29" customWidth="1"/>
-    <col min="20" max="20" width="20.875" style="19" customWidth="1"/>
-    <col min="21" max="21" width="15.75" style="19" customWidth="1"/>
-    <col min="22" max="22" width="17.375" style="19" customWidth="1"/>
-    <col min="23" max="23" width="10.625" style="19" customWidth="1"/>
-    <col min="24" max="24" width="14" style="19" customWidth="1"/>
-    <col min="25" max="25" width="11.625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="20.5" style="19" customWidth="1"/>
-    <col min="27" max="27" width="12.875" style="40" customWidth="1"/>
-    <col min="28" max="28" width="15.75" style="38" customWidth="1"/>
-    <col min="29" max="29" width="15.875" style="20" customWidth="1"/>
-    <col min="30" max="30" width="15.875" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="44" customWidth="1"/>
+    <col min="11" max="11" width="11.75" style="27" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.625" style="27" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="28" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="29" customWidth="1"/>
+    <col min="16" max="18" width="10.5" style="29" customWidth="1"/>
+    <col min="19" max="19" width="13.25" style="29" customWidth="1"/>
+    <col min="20" max="20" width="9" style="27" customWidth="1"/>
+    <col min="21" max="21" width="12.75" style="29" customWidth="1"/>
+    <col min="22" max="22" width="20.875" style="19" customWidth="1"/>
+    <col min="23" max="23" width="15.75" style="19" customWidth="1"/>
+    <col min="24" max="24" width="17.375" style="19" customWidth="1"/>
+    <col min="25" max="25" width="10.625" style="19" customWidth="1"/>
+    <col min="26" max="26" width="14" style="19" customWidth="1"/>
+    <col min="27" max="27" width="11.625" style="19" customWidth="1"/>
+    <col min="28" max="28" width="20.5" style="19" customWidth="1"/>
+    <col min="29" max="29" width="12.875" style="40" customWidth="1"/>
+    <col min="30" max="30" width="15.75" style="38" customWidth="1"/>
+    <col min="31" max="31" width="15.875" style="20" customWidth="1"/>
+    <col min="32" max="32" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>34</v>
       </c>
@@ -953,36 +1036,40 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="31"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
-      <c r="R1" s="16"/>
+      <c r="R1" s="18"/>
       <c r="S1" s="18"/>
-    </row>
-    <row r="2" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="16"/>
+      <c r="U1" s="18"/>
+    </row>
+    <row r="2" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="42"/>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="I2" s="31"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="23"/>
+      <c r="R2" s="25"/>
       <c r="S2" s="25"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T2" s="23"/>
+      <c r="U2" s="25"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>30</v>
       </c>
@@ -991,18 +1078,20 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="31"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="23"/>
+      <c r="R3" s="25"/>
       <c r="S3" s="25"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T3" s="23"/>
+      <c r="U3" s="25"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>32</v>
       </c>
@@ -1014,33 +1103,53 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="31"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
-      <c r="R4" s="16"/>
+      <c r="R4" s="18"/>
       <c r="S4" s="18"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="18"/>
+    </row>
+    <row r="5" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="31"/>
-      <c r="J5" s="22"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="25"/>
-    </row>
-    <row r="6" spans="1:30" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="61"/>
+    </row>
+    <row r="6" spans="1:32" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>3</v>
       </c>
@@ -1069,78 +1178,85 @@
         <v>40</v>
       </c>
       <c r="J6" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="M6" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="N6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="O6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="P6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="Q6" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="R6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="S6" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="30" t="s">
+      <c r="T6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="S6" s="34" t="s">
+      <c r="U6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="V6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="35" t="s">
+      <c r="W6" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="X6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="W6" s="35" t="s">
+      <c r="Y6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="X6" s="35" t="s">
+      <c r="Z6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="35" t="s">
+      <c r="AA6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="Z6" s="35" t="s">
+      <c r="AB6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="41" t="s">
+      <c r="AC6" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="39" t="s">
+      <c r="AD6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="36" t="s">
+      <c r="AE6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AD6" s="37" t="s">
+      <c r="AF6" s="37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="54"/>
-      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AD6"/>
+  <autoFilter ref="A6:AF6"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1302,40 +1418,73 @@
       <c r="B35" s="6"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="A42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="13"/>
+      <c r="A43" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="13"/>
+      <c r="A45" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1346,7 +1495,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1413,6 +1562,20 @@
         <v>44399</v>
       </c>
     </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44403</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20211116 CRE21-019-02	Add $1000 subsidy to SSSCMC - Phase 2: eHS(S)U0015 report
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-015 (HA Scheme)\Front-end (Phase 14 - Enhance eHSU0015 raw data report)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-0XX (SSSCMC $1000)\Front-end (Phase 2 eHSU0015)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Change History" sheetId="31" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AF$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'01-Raw Data'!$A$6:$AG$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -258,6 +258,27 @@
   <si>
     <t xml:space="preserve">Date of Birth </t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE20-019</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top-up subsidy arrangement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient Group</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Patient Group</t>
+  </si>
+  <si>
+    <t>Enrolled before 10 Nov 2021</t>
+  </si>
+  <si>
+    <t>Enrolled or after 10 Nov 2021</t>
   </si>
 </sst>
 </file>
@@ -265,10 +286,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="178" formatCode="0_ "/>
-    <numFmt numFmtId="179" formatCode="[$-13C09]d\ mmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="[$-13C09]d\ mmm\ yyyy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -379,7 +400,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -410,7 +431,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -431,19 +452,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -452,10 +473,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -464,10 +485,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -476,16 +497,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,19 +527,19 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -551,10 +572,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -567,6 +588,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1003,28 +1030,28 @@
     <col min="9" max="9" width="14.5" style="55" customWidth="1"/>
     <col min="10" max="10" width="14.5" style="44" customWidth="1"/>
     <col min="11" max="11" width="11.75" style="27" customWidth="1"/>
-    <col min="12" max="12" width="6.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.625" style="27" customWidth="1"/>
-    <col min="14" max="14" width="9.625" style="28" customWidth="1"/>
-    <col min="15" max="15" width="10.625" style="29" customWidth="1"/>
-    <col min="16" max="18" width="10.5" style="29" customWidth="1"/>
-    <col min="19" max="19" width="13.25" style="29" customWidth="1"/>
-    <col min="20" max="20" width="9" style="27" customWidth="1"/>
-    <col min="21" max="21" width="12.75" style="29" customWidth="1"/>
-    <col min="22" max="22" width="20.875" style="19" customWidth="1"/>
-    <col min="23" max="23" width="15.75" style="19" customWidth="1"/>
-    <col min="24" max="24" width="17.375" style="19" customWidth="1"/>
-    <col min="25" max="25" width="10.625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="14" style="19" customWidth="1"/>
-    <col min="27" max="27" width="11.625" style="19" customWidth="1"/>
-    <col min="28" max="28" width="20.5" style="19" customWidth="1"/>
-    <col min="29" max="29" width="12.875" style="40" customWidth="1"/>
-    <col min="30" max="30" width="15.75" style="38" customWidth="1"/>
-    <col min="31" max="31" width="15.875" style="20" customWidth="1"/>
-    <col min="32" max="32" width="15.875" customWidth="1"/>
+    <col min="12" max="13" width="6.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="27" customWidth="1"/>
+    <col min="15" max="15" width="9.625" style="28" customWidth="1"/>
+    <col min="16" max="16" width="10.625" style="29" customWidth="1"/>
+    <col min="17" max="19" width="10.5" style="29" customWidth="1"/>
+    <col min="20" max="20" width="13.25" style="29" customWidth="1"/>
+    <col min="21" max="21" width="9" style="27" customWidth="1"/>
+    <col min="22" max="22" width="12.75" style="29" customWidth="1"/>
+    <col min="23" max="23" width="20.875" style="19" customWidth="1"/>
+    <col min="24" max="24" width="15.75" style="19" customWidth="1"/>
+    <col min="25" max="25" width="17.375" style="19" customWidth="1"/>
+    <col min="26" max="26" width="10.625" style="19" customWidth="1"/>
+    <col min="27" max="27" width="14" style="19" customWidth="1"/>
+    <col min="28" max="28" width="11.625" style="19" customWidth="1"/>
+    <col min="29" max="29" width="20.5" style="19" customWidth="1"/>
+    <col min="30" max="30" width="12.875" style="40" customWidth="1"/>
+    <col min="31" max="31" width="15.75" style="38" customWidth="1"/>
+    <col min="32" max="32" width="15.875" style="20" customWidth="1"/>
+    <col min="33" max="33" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>34</v>
       </c>
@@ -1039,17 +1066,18 @@
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
       <c r="L1" s="15"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="18"/>
-    </row>
-    <row r="2" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="18"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="18"/>
+    </row>
+    <row r="2" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="42"/>
       <c r="F2" s="22"/>
@@ -1059,17 +1087,18 @@
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
       <c r="L2" s="22"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="24"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="25"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="T2" s="25"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="25"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>30</v>
       </c>
@@ -1081,17 +1110,18 @@
       <c r="J3" s="31"/>
       <c r="K3" s="31"/>
       <c r="L3" s="22"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="25"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="25"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="T3" s="25"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="25"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>32</v>
       </c>
@@ -1106,17 +1136,18 @@
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
       <c r="S4" s="18"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="18"/>
-    </row>
-    <row r="5" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="18"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="18"/>
+    </row>
+    <row r="5" spans="1:33" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="56"/>
       <c r="B5" s="57"/>
       <c r="C5" s="48"/>
@@ -1129,27 +1160,28 @@
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="17"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="58"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="18"/>
       <c r="W5" s="58"/>
       <c r="X5" s="58"/>
       <c r="Y5" s="58"/>
       <c r="Z5" s="58"/>
       <c r="AA5" s="58"/>
       <c r="AB5" s="58"/>
-      <c r="AC5" s="59"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="61"/>
-    </row>
-    <row r="6" spans="1:32" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="60"/>
+      <c r="AF5" s="61"/>
+    </row>
+    <row r="6" spans="1:33" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>3</v>
       </c>
@@ -1186,77 +1218,81 @@
       <c r="L6" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="32" t="s">
+      <c r="O6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="P6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="Q6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="R6" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="33" t="s">
+      <c r="S6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="33" t="s">
+      <c r="T6" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="30" t="s">
+      <c r="U6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="34" t="s">
+      <c r="V6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="W6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="35" t="s">
+      <c r="X6" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="35" t="s">
+      <c r="Y6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" s="35" t="s">
+      <c r="Z6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="35" t="s">
+      <c r="AA6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="AA6" s="35" t="s">
+      <c r="AB6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="AB6" s="35" t="s">
+      <c r="AC6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AC6" s="41" t="s">
+      <c r="AD6" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="AD6" s="39" t="s">
+      <c r="AE6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AE6" s="36" t="s">
+      <c r="AF6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AF6" s="37" t="s">
+      <c r="AG6" s="37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="54"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AF6"/>
+  <autoFilter ref="A6:AG6"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1265,7 +1301,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1486,6 +1522,28 @@
         <v>64</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="64"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="63">
+        <v>1</v>
+      </c>
+      <c r="B48" s="64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="63">
+        <v>2</v>
+      </c>
+      <c r="B49" s="64" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1495,7 +1553,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1576,6 +1634,20 @@
         <v>44403</v>
       </c>
     </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44516</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20220509 CRE22-003	SSSCMC Extension in May 2022
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSU0015-SSSCMC_Transaction_Raw_Data_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swl109\Documents\GitHub\EHS\EHS2019\EHS\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ehp9-fs1\ehs$\Development\InternalChangeControl\2022\CRE22-003 (SSSCMC Extenstion)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -275,16 +275,30 @@
     <t>4. Patient Group</t>
   </si>
   <si>
-    <t>Enrolled before 10 Nov 2021</t>
-  </si>
-  <si>
-    <t>Enrolled or after 10 Nov 2021</t>
+    <t>For patients submitted applications on or before 9 Nov 2021 and subsequently verified</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>For patients submitted applications within 10 Nov 2021 to 9 May 2022 and subsequently verified</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>For patients submitted applications on or after 10 May 2022 and subsequently verified</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE22-003</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSSCMC injection of top-up subsidies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
@@ -1025,7 +1039,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1313,7 +1327,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1556,6 +1570,14 @@
         <v>73</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1565,7 +1587,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1648,7 +1670,7 @@
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>68</v>
@@ -1658,6 +1680,20 @@
       </c>
       <c r="D7" s="10">
         <v>44516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>